<commit_message>
Add invite member in chat room
</commit_message>
<xml_diff>
--- a/docs/data_table.xlsx
+++ b/docs/data_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kataokaryou/Projects/WebOnDocker/2021pf/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kataokaryou/Projects/2021pf/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20100681-2637-D041-AFE3-E7B2847CDF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6903B212-78DF-5643-B0FA-510C09557421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="15800" activeTab="4" xr2:uid="{006DC425-54B7-1E48-9DAD-01E8B14AA901}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="15800" activeTab="5" xr2:uid="{006DC425-54B7-1E48-9DAD-01E8B14AA901}"/>
   </bookViews>
   <sheets>
     <sheet name="サンプル" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="63">
   <si>
     <t>int</t>
     <phoneticPr fontId="1"/>
@@ -4341,7 +4341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10420ED0-48D3-1F4A-8245-4F1C82DDB64E}">
   <dimension ref="B2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
@@ -4643,9 +4643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC252D50-26C3-3F47-A9DE-A8AD9B4E97C6}">
   <dimension ref="B2:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4716,7 +4716,9 @@
       <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G7" s="5" t="s">
         <v>42</v>
       </c>
@@ -4743,7 +4745,9 @@
       <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" s="5" t="s">
         <v>42</v>
       </c>
@@ -4770,7 +4774,9 @@
       <c r="E9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G9" s="5" t="s">
         <v>42</v>
       </c>
@@ -4797,7 +4803,9 @@
       <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" s="5" t="s">
         <v>42</v>
       </c>

</xml_diff>